<commit_message>
commented repositories and ORM
</commit_message>
<xml_diff>
--- a/Doc/_Persos/GZA/Journal_Travail_Guillaume.xlsx
+++ b/Doc/_Persos/GZA/Journal_Travail_Guillaume.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CED397-FAEB-44FD-A52B-941617DC6988}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EC8C5E-D21F-4EDA-BC28-23E66107DC25}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Powwer point présentation intérmédiaire et préparation pour la présentation</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Importation du projet dans intellij</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1245,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
-        <v>43250</v>
+        <v>43221</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>42</v>
@@ -1254,42 +1260,129 @@
       <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="8"/>
+      <c r="A61" s="11">
+        <v>43197</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="8"/>
+      <c r="A62" s="11">
+        <v>43227</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="3"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
       <c r="C63" s="8"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="12"/>
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="12"/>
       <c r="C65" s="8"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="12"/>
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="5" t="s">
+      <c r="A67" s="11"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="11"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="11"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="11"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="11"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="11"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="11"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="11"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="11"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="3"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="3"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="3"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="8"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="9">
-        <f>SUM(C5:C66)</f>
-        <v>57.2</v>
+      <c r="C82" s="9">
+        <f>SUM(C5:C81)</f>
+        <v>59.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction bug not null
</commit_message>
<xml_diff>
--- a/Doc/_Persos/GZA/Journal_Travail_Guillaume.xlsx
+++ b/Doc/_Persos/GZA/Journal_Travail_Guillaume.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EC8C5E-D21F-4EDA-BC28-23E66107DC25}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4922D594-853E-4381-92C2-D2F95297ADEB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,9 +1282,15 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="11"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="8"/>
+      <c r="A63" s="11">
+        <v>43227</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
@@ -1382,7 +1388,7 @@
       </c>
       <c r="C82" s="9">
         <f>SUM(C5:C81)</f>
-        <v>59.7</v>
+        <v>63.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>